<commit_message>
P1A02 files sent to manufactuing review. Added R17, R18, R19, RR20 I2C pullups for reliability and hiher speeds.
</commit_message>
<xml_diff>
--- a/pcb/sensors/Open_Telemetry_digitalSensorShield/Manufacturing/Open_Telemetry_digitalSensorShieldBOM_Generic.xlsx
+++ b/pcb/sensors/Open_Telemetry_digitalSensorShield/Manufacturing/Open_Telemetry_digitalSensorShieldBOM_Generic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Projects\open_telemetry_HW\pcb\sensors\Open_Telemetry_digitalSensorShield\Manufacturing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="8_{FDF07E12-ED3A-4527-A542-B5AA14F99801}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{727972C5-5402-486D-832B-18498EC4EEB0}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{FDF07E12-ED3A-4527-A542-B5AA14F99801}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CD5A9C40-2714-404A-A83C-4C49DCECA7E7}"/>
   <bookViews>
-    <workbookView xWindow="7605" yWindow="1065" windowWidth="21600" windowHeight="11220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2655" yWindow="555" windowWidth="23400" windowHeight="14175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Open_Telemetry_digitalSensorShi" sheetId="1" r:id="rId1"/>
@@ -303,9 +303,6 @@
     <t>https://eu.mouser.com/ProductDetail/Nexperia/BC846BPN115?qs=sGAEpiMZZMvaelWNQAznkcopErTqfTCF</t>
   </si>
   <si>
-    <t>R1, R8, R9, R15, R16</t>
-  </si>
-  <si>
     <t>YAGEO (PHYCOMP)</t>
   </si>
   <si>
@@ -324,9 +321,6 @@
     <t>https://www.mouser.com/Search/Refine.aspx?Keyword=603-RC0201JR-0710KL</t>
   </si>
   <si>
-    <t>R2, R6</t>
-  </si>
-  <si>
     <t>RC0201JR-071KL</t>
   </si>
   <si>
@@ -489,9 +483,6 @@
     <t># Comp.</t>
   </si>
   <si>
-    <t>32/2</t>
-  </si>
-  <si>
     <t>0603</t>
   </si>
   <si>
@@ -510,10 +501,19 @@
     <t>Tot Stock price</t>
   </si>
   <si>
-    <t>Reference: OpenFly Telemetry - OFT001v1 P1A_BOM Rev.:P1A_01</t>
-  </si>
-  <si>
     <t>0201</t>
+  </si>
+  <si>
+    <t>Reference: OpenFly Telemetry - OFT001v1 P1A_BOM Rev.:P1A_02</t>
+  </si>
+  <si>
+    <t>R1, R8, R9, R15, R16, R17, R18</t>
+  </si>
+  <si>
+    <t>R2, R6, R19, R20</t>
+  </si>
+  <si>
+    <t>36/2</t>
   </si>
 </sst>
 </file>
@@ -1017,7 +1017,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1035,6 +1035,9 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -1394,7 +1397,7 @@
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1414,7 +1417,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1455,7 +1458,7 @@
         <v>11</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1478,7 +1481,7 @@
         <v>15</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H5" t="s">
         <v>16</v>
@@ -1519,7 +1522,7 @@
         <v>22</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H6" t="s">
         <v>16</v>
@@ -1765,7 +1768,7 @@
         <v>65</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H12" t="s">
         <v>16</v>
@@ -1806,7 +1809,7 @@
         <v>71</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="H13" t="s">
         <v>16</v>
@@ -1909,39 +1912,39 @@
         <v>0.28999999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>12</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="C16">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
         <v>91</v>
       </c>
-      <c r="C16">
-        <v>5</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>92</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>93</v>
       </c>
-      <c r="F16" t="s">
-        <v>94</v>
-      </c>
       <c r="G16" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H16" t="s">
         <v>16</v>
       </c>
       <c r="I16" t="s">
+        <v>94</v>
+      </c>
+      <c r="J16" t="s">
         <v>95</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>96</v>
-      </c>
-      <c r="K16" t="s">
-        <v>97</v>
       </c>
       <c r="L16">
         <v>0.09</v>
@@ -1955,34 +1958,34 @@
         <v>13</v>
       </c>
       <c r="B17" t="s">
+        <v>160</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
+        <v>91</v>
+      </c>
+      <c r="E17" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" t="s">
         <v>98</v>
       </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17" t="s">
-        <v>92</v>
-      </c>
-      <c r="E17" t="s">
-        <v>99</v>
-      </c>
-      <c r="F17" t="s">
-        <v>100</v>
-      </c>
       <c r="G17" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H17" t="s">
         <v>16</v>
       </c>
       <c r="I17" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J17" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K17" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="L17">
         <v>0.09</v>
@@ -1996,34 +1999,34 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C18">
         <v>2</v>
       </c>
       <c r="D18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H18" t="s">
         <v>16</v>
       </c>
       <c r="I18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K18" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L18">
         <v>0.09</v>
@@ -2037,34 +2040,34 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C19">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E19" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F19" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H19" t="s">
         <v>16</v>
       </c>
       <c r="I19" t="s">
+        <v>109</v>
+      </c>
+      <c r="J19" t="s">
+        <v>110</v>
+      </c>
+      <c r="K19" t="s">
         <v>111</v>
-      </c>
-      <c r="J19" t="s">
-        <v>112</v>
-      </c>
-      <c r="K19" t="s">
-        <v>113</v>
       </c>
       <c r="L19">
         <v>0.09</v>
@@ -2078,34 +2081,34 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
+        <v>113</v>
+      </c>
+      <c r="E20" t="s">
+        <v>114</v>
+      </c>
+      <c r="F20" t="s">
         <v>115</v>
       </c>
-      <c r="E20" t="s">
-        <v>116</v>
-      </c>
-      <c r="F20" t="s">
-        <v>117</v>
-      </c>
       <c r="G20" s="1" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="H20" t="s">
         <v>16</v>
       </c>
       <c r="I20" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="J20" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="K20" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="L20">
         <v>0.09</v>
@@ -2119,19 +2122,19 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C21">
         <v>2</v>
       </c>
       <c r="D21" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" t="s">
+        <v>120</v>
+      </c>
+      <c r="F21" t="s">
         <v>121</v>
-      </c>
-      <c r="E21" t="s">
-        <v>122</v>
-      </c>
-      <c r="F21" t="s">
-        <v>123</v>
       </c>
       <c r="G21" s="1" t="s">
         <v>44</v>
@@ -2140,13 +2143,13 @@
         <v>16</v>
       </c>
       <c r="I21" t="s">
+        <v>122</v>
+      </c>
+      <c r="J21" t="s">
+        <v>123</v>
+      </c>
+      <c r="K21" t="s">
         <v>124</v>
-      </c>
-      <c r="J21" t="s">
-        <v>125</v>
-      </c>
-      <c r="K21" t="s">
-        <v>126</v>
       </c>
       <c r="L21">
         <v>0.82799999999999996</v>
@@ -2160,34 +2163,34 @@
         <v>18</v>
       </c>
       <c r="B22" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
+        <v>126</v>
+      </c>
+      <c r="E22" t="s">
+        <v>127</v>
+      </c>
+      <c r="F22" t="s">
         <v>128</v>
       </c>
-      <c r="E22" t="s">
+      <c r="G22" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="F22" t="s">
-        <v>130</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="H22" t="s">
         <v>16</v>
       </c>
       <c r="I22" t="s">
+        <v>130</v>
+      </c>
+      <c r="J22" t="s">
+        <v>131</v>
+      </c>
+      <c r="K22" t="s">
         <v>132</v>
-      </c>
-      <c r="J22" t="s">
-        <v>133</v>
-      </c>
-      <c r="K22" t="s">
-        <v>134</v>
       </c>
       <c r="L22">
         <v>3.36</v>
@@ -2201,34 +2204,34 @@
         <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
+        <v>134</v>
+      </c>
+      <c r="E23" t="s">
+        <v>135</v>
+      </c>
+      <c r="F23" t="s">
         <v>136</v>
       </c>
-      <c r="E23" t="s">
+      <c r="G23" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="F23" t="s">
-        <v>138</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="H23" t="s">
         <v>16</v>
       </c>
       <c r="I23" t="s">
+        <v>138</v>
+      </c>
+      <c r="J23" t="s">
+        <v>139</v>
+      </c>
+      <c r="K23" t="s">
         <v>140</v>
-      </c>
-      <c r="J23" t="s">
-        <v>141</v>
-      </c>
-      <c r="K23" t="s">
-        <v>142</v>
       </c>
       <c r="L23">
         <v>2.6</v>
@@ -2242,7 +2245,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -2263,40 +2266,40 @@
         <v>20</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C26" s="3">
         <v>2</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>16</v>
       </c>
       <c r="I26" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="K26" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="J26" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>149</v>
-      </c>
       <c r="L26" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="N26" s="3"/>
     </row>
@@ -2305,27 +2308,27 @@
     </row>
     <row r="28" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="C28" s="8" t="s">
         <v>150</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>151</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>152</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
       <c r="H28" s="8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
       <c r="M28" s="8" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
@@ -2335,11 +2338,11 @@
       </c>
       <c r="C29">
         <f>SUM(C5:C23)</f>
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="G29" s="1"/>
       <c r="H29" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="M29">
         <v>25.731999999999999</v>

</xml_diff>

<commit_message>
Corrected the error where BME280 was placed as U1 instead of BMP280 This is the baseline that will be delivered as the P1A prototype card.
</commit_message>
<xml_diff>
--- a/pcb/sensors/Open_Telemetry_digitalSensorShield/Manufacturing/Open_Telemetry_digitalSensorShieldBOM_Generic.xlsx
+++ b/pcb/sensors/Open_Telemetry_digitalSensorShield/Manufacturing/Open_Telemetry_digitalSensorShieldBOM_Generic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jonas\OneDrive\Projects\open_telemetry_HW\pcb\sensors\Open_Telemetry_digitalSensorShield\Manufacturing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{FDF07E12-ED3A-4527-A542-B5AA14F99801}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CD5A9C40-2714-404A-A83C-4C49DCECA7E7}"/>
+  <xr:revisionPtr revIDLastSave="26" documentId="8_{FDF07E12-ED3A-4527-A542-B5AA14F99801}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{CEA09323-499E-4314-923F-600C747CD39F}"/>
   <bookViews>
     <workbookView xWindow="2655" yWindow="555" windowWidth="23400" windowHeight="14175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -411,24 +413,12 @@
     <t>Bosh</t>
   </si>
   <si>
-    <t>BME280</t>
-  </si>
-  <si>
     <t>Barrometic pressure sensor</t>
   </si>
   <si>
-    <t>2.5mmx2.5mmx093mm metal lid LGA</t>
-  </si>
-  <si>
     <t>Open_Telemetry:Bosch_LGA-8_2x2.5mm_P0.65mm_ClockwisePinNumbering</t>
   </si>
   <si>
-    <t>https://ae-bst.resource.bosch.com/media/_tech/media/datasheets/BST-BME280-DS002.pdf</t>
-  </si>
-  <si>
-    <t>https://eu.mouser.com/Search/Refine?Keyword=BME280</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
@@ -514,13 +504,25 @@
   </si>
   <si>
     <t>36/2</t>
+  </si>
+  <si>
+    <t>BMP280</t>
+  </si>
+  <si>
+    <t>2.5mmx2.0mmx095mm metal lid LGA</t>
+  </si>
+  <si>
+    <t>https://www.bosch-sensortec.com/media/boschsensortec/downloads/environmental_sensors_2/pressure_sensors_1/bmp280/bst-bmp280-ds001.pdf</t>
+  </si>
+  <si>
+    <t>https://eu.mouser.com/Search/Refine?Keyword=BMP280</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -663,6 +665,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -973,7 +989,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -1016,8 +1032,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1033,14 +1050,16 @@
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="42"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20 % - Dekorfärg1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20 % - Dekorfärg2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20 % - Dekorfärg3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1070,6 +1089,7 @@
     <cellStyle name="Dekorfärg5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Dekorfärg6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Förklarande text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Hyperlänk" xfId="42" builtinId="8"/>
     <cellStyle name="Indata" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Kontrollcell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Länkad cell" xfId="12" builtinId="24" customBuiltin="1"/>
@@ -1394,10 +1414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:O29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M29" sqref="M29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1417,7 +1437,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -1458,7 +1478,7 @@
         <v>11</v>
       </c>
       <c r="M4" s="7" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1481,7 +1501,7 @@
         <v>15</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H5" t="s">
         <v>16</v>
@@ -1522,7 +1542,7 @@
         <v>22</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H6" t="s">
         <v>16</v>
@@ -1768,7 +1788,7 @@
         <v>65</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H12" t="s">
         <v>16</v>
@@ -1809,7 +1829,7 @@
         <v>71</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H13" t="s">
         <v>16</v>
@@ -1916,8 +1936,8 @@
       <c r="A16">
         <v>12</v>
       </c>
-      <c r="B16" s="10" t="s">
-        <v>159</v>
+      <c r="B16" s="9" t="s">
+        <v>155</v>
       </c>
       <c r="C16">
         <v>7</v>
@@ -1932,7 +1952,7 @@
         <v>93</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H16" t="s">
         <v>16</v>
@@ -1953,12 +1973,12 @@
         <v>0.45</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C17">
         <v>4</v>
@@ -1973,7 +1993,7 @@
         <v>98</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H17" t="s">
         <v>16</v>
@@ -1994,7 +2014,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>14</v>
       </c>
@@ -2014,7 +2034,7 @@
         <v>103</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H18" t="s">
         <v>16</v>
@@ -2035,7 +2055,7 @@
         <v>0.18</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>15</v>
       </c>
@@ -2055,7 +2075,7 @@
         <v>108</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H19" t="s">
         <v>16</v>
@@ -2076,7 +2096,7 @@
         <v>0.36</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>16</v>
       </c>
@@ -2096,7 +2116,7 @@
         <v>115</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="H20" t="s">
         <v>16</v>
@@ -2117,7 +2137,7 @@
         <v>0.09</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>17</v>
       </c>
@@ -2158,7 +2178,7 @@
         <v>1.6559999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>18</v>
       </c>
@@ -2172,66 +2192,66 @@
         <v>126</v>
       </c>
       <c r="E22" t="s">
+        <v>158</v>
+      </c>
+      <c r="F22" t="s">
         <v>127</v>
       </c>
-      <c r="F22" t="s">
-        <v>128</v>
-      </c>
       <c r="G22" s="1" t="s">
-        <v>129</v>
+        <v>159</v>
       </c>
       <c r="H22" t="s">
         <v>16</v>
       </c>
       <c r="I22" t="s">
-        <v>130</v>
-      </c>
-      <c r="J22" t="s">
-        <v>131</v>
-      </c>
-      <c r="K22" t="s">
-        <v>132</v>
-      </c>
-      <c r="L22">
-        <v>3.36</v>
-      </c>
-      <c r="M22">
-        <v>3.36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+      <c r="J22" s="11" t="s">
+        <v>160</v>
+      </c>
+      <c r="K22" s="11" t="s">
+        <v>161</v>
+      </c>
+      <c r="L22" s="12">
+        <v>2.76</v>
+      </c>
+      <c r="M22" s="12">
+        <v>2.76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>19</v>
       </c>
       <c r="B23" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E23" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="F23" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="H23" t="s">
         <v>16</v>
       </c>
       <c r="I23" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="J23" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="K23" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="L23">
         <v>2.6</v>
@@ -2240,12 +2260,12 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="G24" s="1"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -2261,12 +2281,12 @@
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>20</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C26" s="3">
         <v>2</v>
@@ -2275,64 +2295,65 @@
         <v>91</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="G26" s="4" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>16</v>
       </c>
       <c r="I26" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="K26" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="L26" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="M26" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="N26" s="3"/>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G27" s="1"/>
+      <c r="O27" s="12"/>
+    </row>
+    <row r="28" spans="1:15" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B28" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="J26" s="3" t="s">
+      <c r="C28" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="K26" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="L26" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="M26" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="N26" s="3"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G27" s="1"/>
-    </row>
-    <row r="28" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>149</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>150</v>
       </c>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
       <c r="G28" s="8"/>
       <c r="H28" s="8" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="I28" s="8"/>
       <c r="J28" s="8"/>
       <c r="K28" s="8"/>
       <c r="L28" s="8"/>
       <c r="M28" s="8" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="9"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A29" s="10"/>
       <c r="B29">
         <v>19</v>
       </c>
@@ -2342,17 +2363,22 @@
       </c>
       <c r="G29" s="1"/>
       <c r="H29" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="M29">
-        <v>25.731999999999999</v>
+        <f>SUM(M5:M23)</f>
+        <v>25.131999999999998</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A28:A29"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="J22" r:id="rId1" xr:uid="{9049F74C-6EB9-45A0-B72C-8B5FAE4006A2}"/>
+    <hyperlink ref="K22" r:id="rId2" xr:uid="{C2F73CE5-2FCD-48F3-8E06-850E4479E0A2}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>